<commit_message>
auth fixings, logging and enchasements
</commit_message>
<xml_diff>
--- a/static/tmp/statistic.xlsx
+++ b/static/tmp/statistic.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="bot" sheetId="1" r:id="rId1" state="visible"/>
+    <sheet name="quests" sheetId="2" r:id="rId2" state="visible"/>
   </sheets>
   <definedNames/>
   <calcPr iterateCount="100" refMode="A1" iterateDelta="0.001"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>coffee_test</t>
   </si>
@@ -43,6 +44,15 @@
   </si>
   <si>
     <t>ФИО водителя</t>
+  </si>
+  <si>
+    <t>TESTPHONE</t>
+  </si>
+  <si>
+    <t>Не определен</t>
+  </si>
+  <si>
+    <t>TESTPHONE2</t>
   </si>
 </sst>
 </file>
@@ -81,11 +91,14 @@
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="1" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="14">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -417,7 +430,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -466,6 +479,479 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>42507.720659722225</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>42507.7202662037</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>42494.91145833333</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
+        <v>42494.90429398148</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>42494.90019675926</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>42494.89875</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2">
+        <v>42494.896006944444</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2">
+        <v>42494.89313657407</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2">
+        <v>42494.885150462964</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
+        <v>42494.88377314815</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2">
+        <v>42494.88337962963</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2">
+        <v>42494.852685185186</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2">
+        <v>42494.84486111111</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2">
+        <v>42494.84443287037</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2">
+        <v>42494.80725694445</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2">
+        <v>42494.806701388894</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2">
+        <v>42494.801574074074</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2">
+        <v>42494.79256944444</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2">
+        <v>42494.78834490741</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2">
+        <v>42494.78113425926</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2">
+        <v>42491.76986111111</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2">
+        <v>42491.76907407407</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="2">
+        <v>42491.76650462963</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="2">
+        <v>42489.79824074074</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="2">
+        <v>42489.78869212963</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2">
+        <v>42489.77340277778</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2">
+        <v>42489.74018518519</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="2">
+        <v>42487.82724537037</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="2">
+        <v>42487.797685185185</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="2">
+        <v>42487.79725694444</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="2">
+        <v>42487.79686342593</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="2">
+        <v>42487.79619212963</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="2">
+        <v>42487.79553240741</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2">
+        <v>42487.79430555555</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="2">
+        <v>42487.793587962966</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="2">
+        <v>42487.792962962965</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="2">
+        <v>42487.790856481486</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="2">
+        <v>42487.78266203703</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="2">
+        <v>42487.780752314815</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="2">
+        <v>42487.779178240744</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="2">
+        <v>42487.77693287037</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="2">
+        <v>42487.739745370374</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="2">
+        <v>42487.739699074074</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -475,4 +961,28 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>